<commit_message>
playwright headless done init
</commit_message>
<xml_diff>
--- a/tablasResultados.xlsx
+++ b/tablasResultados.xlsx
@@ -292,7 +292,145 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="47">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color theme="1"/>
+        </top>
+        <bottom style="medium">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -591,40 +729,10 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="medium">
           <color theme="1"/>
         </top>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="6"/>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border outline="0">
@@ -10113,10 +10221,22 @@
     <tableColumn id="3" name="CPU %2"/>
     <tableColumn id="4" name="RAM Inicial"/>
     <tableColumn id="5" name="RAM final"/>
-    <tableColumn id="8" name="Columna1" dataDxfId="39">
+    <tableColumn id="8" name="Columna1" dataDxfId="46">
       <calculatedColumnFormula>Tabla1[[#This Row],[RAM final]]-Tabla1[[#This Row],[RAM Inicial]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="time Ejec"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla10" displayName="Tabla10" ref="K72:M92" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3" headerRowBorderDxfId="7" tableBorderDxfId="8">
+  <autoFilter ref="K72:M92"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="#" dataDxfId="6"/>
+    <tableColumn id="2" name="CPU GHz" dataDxfId="5"/>
+    <tableColumn id="3" name="CPU %" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10127,7 +10247,7 @@
   <autoFilter ref="K4:N24"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Ejecución"/>
-    <tableColumn id="8" name="RAM" dataDxfId="38"/>
+    <tableColumn id="8" name="RAM" dataDxfId="45"/>
     <tableColumn id="9" name="CPU %"/>
     <tableColumn id="6" name="Time"/>
   </tableColumns>
@@ -10136,20 +10256,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="K26:N46" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="K26:N46" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41">
   <autoFilter ref="K26:N46"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="33"/>
-    <tableColumn id="2" name="RAM USED" dataDxfId="32"/>
-    <tableColumn id="3" name="CPU %" dataDxfId="31"/>
-    <tableColumn id="4" name="TIME/s" dataDxfId="30"/>
+    <tableColumn id="1" name="#" dataDxfId="40"/>
+    <tableColumn id="2" name="RAM USED" dataDxfId="39"/>
+    <tableColumn id="3" name="CPU %" dataDxfId="38"/>
+    <tableColumn id="4" name="TIME/s" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="B49:H69" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="B49:H69" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35" tableBorderDxfId="34">
   <autoFilter ref="B49:H69"/>
   <tableColumns count="7">
     <tableColumn id="1" name="#"/>
@@ -10167,7 +10287,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="B72:H92" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="B72:H92" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
   <autoFilter ref="B72:H92"/>
   <tableColumns count="7">
     <tableColumn id="1" name="#"/>
@@ -10185,14 +10305,14 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla57" displayName="Tabla57" ref="B95:G115" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="21" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla57" displayName="Tabla57" ref="B95:G115" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="30">
   <autoFilter ref="B95:G115"/>
   <tableColumns count="6">
     <tableColumn id="1" name="#"/>
     <tableColumn id="3" name="CPU"/>
     <tableColumn id="4" name="RAM Inicial"/>
     <tableColumn id="5" name="RAM final"/>
-    <tableColumn id="6" name="RAM USED" dataDxfId="20">
+    <tableColumn id="6" name="RAM USED" dataDxfId="29">
       <calculatedColumnFormula>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="TIME/ms"/>
@@ -10202,14 +10322,14 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla578" displayName="Tabla578" ref="B118:G138" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla578" displayName="Tabla578" ref="B118:G138" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="26" tableBorderDxfId="27">
   <autoFilter ref="B118:G138"/>
   <tableColumns count="6">
     <tableColumn id="1" name="#"/>
     <tableColumn id="3" name="CPU %"/>
     <tableColumn id="4" name="RAM Inicial"/>
     <tableColumn id="5" name="RAM final"/>
-    <tableColumn id="6" name="RAM USED" dataDxfId="8">
+    <tableColumn id="6" name="RAM USED" dataDxfId="17">
       <calculatedColumnFormula>Tabla578[[#This Row],[RAM final]]-Tabla578[[#This Row],[RAM Inicial]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="TIME/ms"/>
@@ -10219,17 +10339,17 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="K95:N115" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="K95:N115" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" headerRowBorderDxfId="22" tableBorderDxfId="23">
   <autoFilter ref="K95:N115"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="12"/>
-    <tableColumn id="2" name="CPU %" dataDxfId="11">
+    <tableColumn id="1" name="#" dataDxfId="21"/>
+    <tableColumn id="2" name="CPU %" dataDxfId="20">
       <calculatedColumnFormula>Tabla57[[#This Row],[CPU]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="TIME/S" dataDxfId="10">
+    <tableColumn id="4" name="TIME/S" dataDxfId="19">
       <calculatedColumnFormula>Tabla57[[#This Row],[TIME/ms]]/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="RAM USED" dataDxfId="9">
+    <tableColumn id="5" name="RAM USED" dataDxfId="18">
       <calculatedColumnFormula>Tabla57[[#This Row],[RAM USED]]/1048576</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10238,17 +10358,17 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla810" displayName="Tabla810" ref="K118:N138" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla810" displayName="Tabla810" ref="K118:N138" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14">
   <autoFilter ref="K118:N138"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="3"/>
-    <tableColumn id="2" name="CPU %" dataDxfId="2">
+    <tableColumn id="1" name="#" dataDxfId="12"/>
+    <tableColumn id="2" name="CPU %" dataDxfId="11">
       <calculatedColumnFormula>Tabla578[[#This Row],[CPU %]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="TIME/S" dataDxfId="1">
+    <tableColumn id="4" name="TIME/S" dataDxfId="10">
       <calculatedColumnFormula>Tabla578[[#This Row],[TIME/ms]]/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="RAM USED" dataDxfId="0">
+    <tableColumn id="5" name="RAM USED" dataDxfId="9">
       <calculatedColumnFormula>Tabla578[[#This Row],[RAM USED]]/1048576</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10640,8 +10760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:N138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H93" workbookViewId="0">
-      <selection activeCell="X113" sqref="X113"/>
+    <sheetView tabSelected="1" topLeftCell="K98" workbookViewId="0">
+      <selection activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12857,7 +12977,6 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="72" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B72" s="14" t="s">
         <v>10</v>
@@ -12880,13 +12999,13 @@
       <c r="H72" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K72" s="1" t="s">
+      <c r="K72" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="L72" s="1" t="s">
+      <c r="L72" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M72" s="1" t="s">
+      <c r="M72" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -13517,7 +13636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B92">
         <v>20</v>
       </c>
@@ -13540,13 +13659,13 @@
       <c r="H92">
         <v>12</v>
       </c>
-      <c r="K92" s="4">
+      <c r="K92" s="15">
         <v>20</v>
       </c>
-      <c r="L92" s="4">
+      <c r="L92" s="15">
         <v>3.13</v>
       </c>
-      <c r="M92" s="4">
+      <c r="M92" s="15">
         <v>5</v>
       </c>
     </row>
@@ -13599,7 +13718,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>228159488</v>
       </c>
-      <c r="G96" s="16">
+      <c r="G96">
         <v>12179225</v>
       </c>
       <c r="K96" s="2">
@@ -13635,7 +13754,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>142442496</v>
       </c>
-      <c r="G97" s="16">
+      <c r="G97">
         <v>12126218</v>
       </c>
       <c r="K97" s="3">
@@ -13671,7 +13790,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>167600128</v>
       </c>
-      <c r="G98" s="16">
+      <c r="G98">
         <v>12104940</v>
       </c>
       <c r="K98" s="2">
@@ -13707,7 +13826,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>245547008</v>
       </c>
-      <c r="G99" s="16">
+      <c r="G99">
         <v>12050825</v>
       </c>
       <c r="K99" s="3">
@@ -13736,14 +13855,14 @@
       <c r="D100">
         <v>16191029248</v>
       </c>
-      <c r="E100" s="17">
+      <c r="E100">
         <v>16359321600</v>
       </c>
       <c r="F100">
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>168292352</v>
       </c>
-      <c r="G100" s="16">
+      <c r="G100">
         <v>12132151</v>
       </c>
       <c r="K100" s="2">
@@ -13779,7 +13898,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>170143744</v>
       </c>
-      <c r="G101" s="16">
+      <c r="G101">
         <v>12172336</v>
       </c>
       <c r="K101" s="3">
@@ -13815,7 +13934,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>138268672</v>
       </c>
-      <c r="G102" s="16">
+      <c r="G102">
         <v>12053261</v>
       </c>
       <c r="K102" s="2">
@@ -13851,7 +13970,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>185868288</v>
       </c>
-      <c r="G103" s="16">
+      <c r="G103">
         <v>12095738</v>
       </c>
       <c r="K103" s="3">
@@ -13887,7 +14006,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>165638144</v>
       </c>
-      <c r="G104" s="16">
+      <c r="G104">
         <v>12139102</v>
       </c>
       <c r="K104" s="2">
@@ -13916,14 +14035,14 @@
       <c r="D105">
         <v>16137093120</v>
       </c>
-      <c r="E105" s="17">
+      <c r="E105">
         <v>16308903936</v>
       </c>
       <c r="F105">
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>171810816</v>
       </c>
-      <c r="G105" s="16">
+      <c r="G105">
         <v>12661537</v>
       </c>
       <c r="K105" s="3">
@@ -13959,7 +14078,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>129667072</v>
       </c>
-      <c r="G106" s="16">
+      <c r="G106">
         <v>12400420</v>
       </c>
       <c r="K106" s="2">
@@ -13995,7 +14114,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>205893632</v>
       </c>
-      <c r="G107" s="16">
+      <c r="G107">
         <v>12438353</v>
       </c>
       <c r="K107" s="3">
@@ -14031,7 +14150,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>168505344</v>
       </c>
-      <c r="G108" s="16">
+      <c r="G108">
         <v>12621905</v>
       </c>
       <c r="K108" s="2">
@@ -14067,7 +14186,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>175771648</v>
       </c>
-      <c r="G109" s="16">
+      <c r="G109">
         <v>12482345</v>
       </c>
       <c r="K109" s="3">
@@ -14103,7 +14222,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>173719552</v>
       </c>
-      <c r="G110" s="16">
+      <c r="G110">
         <v>12423661</v>
       </c>
       <c r="K110" s="2">
@@ -14139,7 +14258,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>179150848</v>
       </c>
-      <c r="G111" s="16">
+      <c r="G111">
         <v>12244723</v>
       </c>
       <c r="K111" s="3">
@@ -14175,7 +14294,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>172072960</v>
       </c>
-      <c r="G112" s="16">
+      <c r="G112">
         <v>12418507</v>
       </c>
       <c r="K112" s="2">
@@ -14211,7 +14330,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>174968832</v>
       </c>
-      <c r="G113" s="16">
+      <c r="G113">
         <v>12365284</v>
       </c>
       <c r="K113" s="3">
@@ -14247,7 +14366,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>183623680</v>
       </c>
-      <c r="G114" s="16">
+      <c r="G114">
         <v>12403503</v>
       </c>
       <c r="K114" s="2">
@@ -14283,7 +14402,7 @@
         <f>Tabla57[[#This Row],[RAM final]]-Tabla57[[#This Row],[RAM Inicial]]</f>
         <v>164278272</v>
       </c>
-      <c r="G115" s="16">
+      <c r="G115">
         <v>19386008</v>
       </c>
       <c r="K115" s="15">
@@ -15058,7 +15177,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="9">
+  <tableParts count="10">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
@@ -15068,6 +15187,7 @@
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
     <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>